<commit_message>
add basic report functions
</commit_message>
<xml_diff>
--- a/Reports/template.xlsx
+++ b/Reports/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t xml:space="preserve">Spielbericht</t>
   </si>
@@ -67,6 +67,9 @@
     <t xml:space="preserve">Spielklasse</t>
   </si>
   <si>
+    <t xml:space="preserve">Mixed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Datum</t>
   </si>
   <si>
@@ -107,12 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">Protokollführer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Göttinger PC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KG Ressort Polo</t>
   </si>
   <si>
     <t xml:space="preserve">No.</t>
@@ -373,167 +370,167 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -620,9 +617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>450720</xdr:colOff>
+      <xdr:colOff>450360</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -636,7 +633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="20160"/>
-          <a:ext cx="1175760" cy="846360"/>
+          <a:ext cx="1175400" cy="846000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -659,10 +656,10 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="X28" activeCellId="0" sqref="X28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6"/>
@@ -716,16 +713,16 @@
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="8" t="str">
+      <c r="L2" s="8" t="n">
         <f aca="false">B22</f>
-        <v>Göttinger PC</v>
+        <v>0</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
-      <c r="P2" s="8" t="str">
+      <c r="P2" s="8" t="n">
         <f aca="false">F22</f>
-        <v>KG Ressort Polo</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="7" t="s">
@@ -828,8 +825,12 @@
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="17"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
@@ -861,18 +862,18 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" s="16"/>
       <c r="I9" s="12"/>
@@ -892,10 +893,10 @@
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="22"/>
@@ -936,7 +937,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -959,12 +960,12 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -1005,12 +1006,12 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
@@ -1051,12 +1052,12 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
@@ -1097,7 +1098,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1157,17 +1158,13 @@
       <c r="A22" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>29</v>
-      </c>
+      <c r="B22" s="25"/>
       <c r="C22" s="26"/>
       <c r="D22" s="27"/>
       <c r="E22" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="28" t="s">
-        <v>30</v>
-      </c>
+      <c r="F22" s="28"/>
       <c r="G22" s="29"/>
       <c r="I22" s="12"/>
       <c r="J22" s="13"/>
@@ -1184,23 +1181,23 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>31</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>32</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="G23" s="30" t="s">
         <v>32</v>
-      </c>
-      <c r="G23" s="30" t="s">
-        <v>33</v>
       </c>
       <c r="I23" s="12"/>
       <c r="J23" s="13"/>
@@ -1358,7 +1355,7 @@
       <c r="L29" s="16"/>
       <c r="M29" s="33"/>
       <c r="N29" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O29" s="34"/>
       <c r="P29" s="33"/>
@@ -1379,9 +1376,9 @@
       </c>
       <c r="F30" s="32"/>
       <c r="G30" s="32"/>
-      <c r="I30" s="35" t="str">
+      <c r="I30" s="35" t="n">
         <f aca="false">L2</f>
-        <v>Göttinger PC</v>
+        <v>0</v>
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
@@ -1393,9 +1390,9 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
       <c r="S30" s="16"/>
-      <c r="T30" s="36" t="str">
+      <c r="T30" s="36" t="n">
         <f aca="false">P2</f>
-        <v>KG Ressort Polo</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1414,7 +1411,7 @@
       <c r="L31" s="37"/>
       <c r="M31" s="38"/>
       <c r="N31" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O31" s="39"/>
       <c r="P31" s="38"/>
@@ -1468,7 +1465,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="16"/>
       <c r="B34" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
@@ -1484,7 +1481,7 @@
       <c r="O34" s="16"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R34" s="16"/>
       <c r="S34" s="16"/>
@@ -1494,12 +1491,12 @@
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D35" s="40"/>
       <c r="E35" s="16"/>
       <c r="F35" s="40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G35" s="40"/>
       <c r="H35" s="16"/>
@@ -1507,12 +1504,12 @@
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
       <c r="L35" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M35" s="40"/>
       <c r="N35" s="40"/>
       <c r="O35" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P35" s="40"/>
       <c r="Q35" s="40"/>
@@ -1522,7 +1519,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="41"/>
       <c r="C36" s="31"/>
@@ -1532,7 +1529,7 @@
       <c r="G36" s="31"/>
       <c r="H36" s="16"/>
       <c r="I36" s="41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J36" s="41"/>
       <c r="K36" s="41"/>
@@ -1543,7 +1540,7 @@
       <c r="P36" s="31"/>
       <c r="Q36" s="31"/>
       <c r="R36" s="41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S36" s="41"/>
       <c r="T36" s="41"/>

</xml_diff>

<commit_message>
new date for template. ignore teamnames with "platz"
</commit_message>
<xml_diff>
--- a/Reports/template.xlsx
+++ b/Reports/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/GIT/Swiss-Tournament/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEF160E-FF6E-FB41-AF46-4DCE8DBCAAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B092C00-6DE6-3F44-AAEA-E77518348C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -156,10 +156,10 @@
  Spiel</t>
   </si>
   <si>
-    <t>3. Würzburger Poloturnier</t>
-  </si>
-  <si>
     <t>2min</t>
+  </si>
+  <si>
+    <t>4. Würzburger Poloturnier</t>
   </si>
 </sst>
 </file>
@@ -429,50 +429,50 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -927,7 +927,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -954,20 +954,20 @@
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="5"/>
@@ -975,32 +975,32 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44" t="str">
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32" t="str">
         <f>IF(ISBLANK(B22),"",B22)</f>
         <v/>
       </c>
-      <c r="M2" s="44"/>
+      <c r="M2" s="32"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
-      <c r="P2" s="44" t="str">
+      <c r="P2" s="32" t="str">
         <f>IF(ISBLANK(F22),"",F22)</f>
         <v/>
       </c>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="Q2" s="32"/>
+      <c r="R2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="7" t="s">
@@ -1018,8 +1018,8 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
@@ -1038,8 +1038,8 @@
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="11"/>
@@ -1052,8 +1052,8 @@
       <c r="K5" s="13"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="11"/>
@@ -1080,8 +1080,8 @@
       <c r="K6" s="13"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="11"/>
@@ -1089,23 +1089,23 @@
       <c r="T6" s="13"/>
     </row>
     <row r="7" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16">
         <v>1</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="35"/>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
       <c r="K7" s="13"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="11"/>
@@ -1119,8 +1119,8 @@
       <c r="K8" s="13"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="11"/>
@@ -1148,8 +1148,8 @@
       <c r="K9" s="13"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="11"/>
@@ -1157,13 +1157,13 @@
       <c r="T9" s="13"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="18"/>
@@ -1173,8 +1173,8 @@
       <c r="K10" s="13"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="11"/>
@@ -1194,8 +1194,8 @@
       <c r="K11" s="13"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="11"/>
@@ -1208,8 +1208,8 @@
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="I12" s="11"/>
@@ -1217,8 +1217,8 @@
       <c r="K12" s="13"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="11"/>
@@ -1242,8 +1242,8 @@
       <c r="K13" s="13"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="11"/>
@@ -1251,11 +1251,11 @@
       <c r="T13" s="13"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="I14" s="11"/>
@@ -1263,8 +1263,8 @@
       <c r="K14" s="13"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="11"/>
@@ -1288,8 +1288,8 @@
       <c r="K15" s="13"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="11"/>
@@ -1297,11 +1297,11 @@
       <c r="T15" s="13"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="I16" s="11"/>
@@ -1309,8 +1309,8 @@
       <c r="K16" s="13"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="11"/>
@@ -1334,8 +1334,8 @@
       <c r="K17" s="13"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="11"/>
@@ -1343,11 +1343,11 @@
       <c r="T17" s="13"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="I18" s="11"/>
@@ -1355,8 +1355,8 @@
       <c r="K18" s="13"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="11"/>
@@ -1378,8 +1378,8 @@
       <c r="K19" s="13"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="11"/>
@@ -1387,9 +1387,9 @@
       <c r="T19" s="13"/>
     </row>
     <row r="20" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
@@ -1399,8 +1399,8 @@
       <c r="K20" s="13"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="11"/>
@@ -1413,8 +1413,8 @@
       <c r="K21" s="13"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="11"/>
@@ -1438,8 +1438,8 @@
       <c r="K22" s="13"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="11"/>
@@ -1450,10 +1450,10 @@
       <c r="A23" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="30"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="26" t="s">
         <v>29</v>
       </c>
@@ -1471,8 +1471,8 @@
       <c r="K23" s="13"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="11"/>
@@ -1481,8 +1481,8 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1492,8 +1492,8 @@
       <c r="K24" s="13"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="11"/>
@@ -1502,8 +1502,8 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1513,8 +1513,8 @@
       <c r="K25" s="13"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="11"/>
@@ -1523,8 +1523,8 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1534,8 +1534,8 @@
       <c r="K26" s="13"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="11"/>
@@ -1544,8 +1544,8 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1555,8 +1555,8 @@
       <c r="K27" s="13"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="11"/>
@@ -1565,8 +1565,8 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1576,8 +1576,8 @@
       <c r="K28" s="13"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="11"/>
@@ -1586,8 +1586,8 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1596,12 +1596,12 @@
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
       <c r="L29" s="14"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="38" t="s">
+      <c r="M29" s="39"/>
+      <c r="N29" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="O29" s="38"/>
-      <c r="P29" s="34"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="39"/>
       <c r="Q29" s="14"/>
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
@@ -1609,8 +1609,8 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1619,10 +1619,10 @@
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="34"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="39"/>
       <c r="Q30" s="14"/>
       <c r="R30" s="14"/>
       <c r="S30" s="14"/>
@@ -1630,8 +1630,8 @@
     </row>
     <row r="31" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1640,12 +1640,12 @@
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="36" t="s">
+      <c r="M31" s="41"/>
+      <c r="N31" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="O31" s="36"/>
-      <c r="P31" s="35"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="41"/>
       <c r="Q31" s="14"/>
       <c r="R31" s="29"/>
       <c r="S31" s="29"/>
@@ -1653,8 +1653,8 @@
     </row>
     <row r="32" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1663,10 +1663,10 @@
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="29"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="35"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="41"/>
       <c r="Q32" s="29"/>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
@@ -1674,8 +1674,8 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1721,134 +1721,187 @@
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="33"/>
+      <c r="D35" s="43"/>
       <c r="E35" s="14"/>
-      <c r="F35" s="33" t="s">
+      <c r="F35" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="33"/>
+      <c r="G35" s="43"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
-      <c r="L35" s="33" t="s">
+      <c r="L35" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33" t="s">
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43"/>
       <c r="R35" s="14"/>
       <c r="S35" s="14"/>
       <c r="T35" s="14"/>
     </row>
     <row r="36" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="14"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
       <c r="H36" s="14"/>
-      <c r="I36" s="31" t="s">
+      <c r="I36" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="31" t="s">
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37"/>
+      <c r="Q36" s="37"/>
+      <c r="R36" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="S36" s="31"/>
-      <c r="T36" s="31"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="14"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
       <c r="H37" s="14"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="31"/>
-      <c r="S37" s="31"/>
-      <c r="T37" s="31"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="14"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
       <c r="H38" s="14"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="31"/>
-      <c r="S38" s="31"/>
-      <c r="T38" s="31"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="14"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
       <c r="H39" s="14"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="31"/>
-      <c r="S39" s="31"/>
-      <c r="T39" s="31"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="I1:T1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="O36:Q39"/>
+    <mergeCell ref="R36:T39"/>
+    <mergeCell ref="A36:B39"/>
+    <mergeCell ref="C36:D39"/>
+    <mergeCell ref="F36:G39"/>
+    <mergeCell ref="I36:K39"/>
+    <mergeCell ref="L36:N39"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="P29:P30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="N31:O32"/>
+    <mergeCell ref="P31:P32"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="N29:O30"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="N5:O5"/>
@@ -1856,64 +1909,11 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="N29:O30"/>
-    <mergeCell ref="P29:P30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="M31:M32"/>
-    <mergeCell ref="N31:O32"/>
-    <mergeCell ref="P31:P32"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="O35:Q35"/>
-    <mergeCell ref="O36:Q39"/>
-    <mergeCell ref="R36:T39"/>
-    <mergeCell ref="A36:B39"/>
-    <mergeCell ref="C36:D39"/>
-    <mergeCell ref="F36:G39"/>
-    <mergeCell ref="I36:K39"/>
-    <mergeCell ref="L36:N39"/>
+    <mergeCell ref="I1:T1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:T2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5625" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>